<commit_message>
commit changes in data and logic
</commit_message>
<xml_diff>
--- a/output/alm_gap_report.xlsx
+++ b/output/alm_gap_report.xlsx
@@ -526,16 +526,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>36570889</v>
+        <v>40097834</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>17650714</v>
       </c>
       <c r="D5" t="n">
-        <v>36570889</v>
+        <v>22447120</v>
       </c>
       <c r="E5" t="n">
-        <v>49663724</v>
+        <v>35539955</v>
       </c>
     </row>
     <row r="6">
@@ -545,16 +545,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>39831073</v>
+        <v>50865822</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>912681</v>
       </c>
       <c r="D6" t="n">
-        <v>39831073</v>
+        <v>49953141</v>
       </c>
       <c r="E6" t="n">
-        <v>89494797</v>
+        <v>85493096</v>
       </c>
     </row>
     <row r="7">
@@ -564,16 +564,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>157575087</v>
+        <v>181047468</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>22049274</v>
       </c>
       <c r="D7" t="n">
-        <v>157575087</v>
+        <v>158998194</v>
       </c>
       <c r="E7" t="n">
-        <v>247069884</v>
+        <v>244491290</v>
       </c>
     </row>
     <row r="8">
@@ -583,16 +583,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>137703222</v>
       </c>
       <c r="C8" t="n">
-        <v>39973229</v>
+        <v>95188050</v>
       </c>
       <c r="D8" t="n">
-        <v>-39973229</v>
+        <v>42515172</v>
       </c>
       <c r="E8" t="n">
-        <v>207096655</v>
+        <v>287006462</v>
       </c>
     </row>
     <row r="9">
@@ -602,16 +602,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>48148807</v>
       </c>
       <c r="C9" t="n">
-        <v>12898804</v>
+        <v>67867558</v>
       </c>
       <c r="D9" t="n">
-        <v>-12898804</v>
+        <v>-19718751</v>
       </c>
       <c r="E9" t="n">
-        <v>194197851</v>
+        <v>267287711</v>
       </c>
     </row>
     <row r="10">
@@ -624,13 +624,13 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>34786904</v>
+        <v>96621244</v>
       </c>
       <c r="D10" t="n">
-        <v>-34786904</v>
+        <v>-96621244</v>
       </c>
       <c r="E10" t="n">
-        <v>159410947</v>
+        <v>170666467</v>
       </c>
     </row>
     <row r="11">
@@ -743,16 +743,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>31674996</v>
+        <v>48871432</v>
       </c>
       <c r="C4" t="n">
         <v>78670</v>
       </c>
       <c r="D4" t="n">
-        <v>31596326</v>
+        <v>48792762</v>
       </c>
       <c r="E4" t="n">
-        <v>37992989</v>
+        <v>55189425</v>
       </c>
     </row>
     <row r="5">
@@ -762,16 +762,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>55144424</v>
+        <v>90462007</v>
       </c>
       <c r="C5" t="n">
-        <v>3473494</v>
+        <v>33520374</v>
       </c>
       <c r="D5" t="n">
-        <v>51670930</v>
+        <v>56941633</v>
       </c>
       <c r="E5" t="n">
-        <v>89663919</v>
+        <v>112131058</v>
       </c>
     </row>
     <row r="6">
@@ -781,16 +781,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>61290623</v>
+        <v>67725781</v>
       </c>
       <c r="C6" t="n">
-        <v>6487129</v>
+        <v>31488965</v>
       </c>
       <c r="D6" t="n">
-        <v>54803494</v>
+        <v>36236816</v>
       </c>
       <c r="E6" t="n">
-        <v>144467413</v>
+        <v>148367874</v>
       </c>
     </row>
     <row r="7">
@@ -800,16 +800,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>92353723</v>
+        <v>128817688</v>
       </c>
       <c r="C7" t="n">
-        <v>10284757</v>
+        <v>46327208</v>
       </c>
       <c r="D7" t="n">
-        <v>82068966</v>
+        <v>82490480</v>
       </c>
       <c r="E7" t="n">
-        <v>226536379</v>
+        <v>230858354</v>
       </c>
     </row>
     <row r="8">
@@ -819,16 +819,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>99349448</v>
       </c>
       <c r="C8" t="n">
-        <v>30797010</v>
+        <v>101287781</v>
       </c>
       <c r="D8" t="n">
-        <v>-30797010</v>
+        <v>-1938333</v>
       </c>
       <c r="E8" t="n">
-        <v>195739369</v>
+        <v>228920021</v>
       </c>
     </row>
     <row r="9">
@@ -838,16 +838,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>29123514</v>
       </c>
       <c r="C9" t="n">
-        <v>13028932</v>
+        <v>37233029</v>
       </c>
       <c r="D9" t="n">
-        <v>-13028932</v>
+        <v>-8109515</v>
       </c>
       <c r="E9" t="n">
-        <v>182710437</v>
+        <v>220810506</v>
       </c>
     </row>
     <row r="10">
@@ -860,13 +860,13 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>23299490</v>
+        <v>50144039</v>
       </c>
       <c r="D10" t="n">
-        <v>-23299490</v>
+        <v>-50144039</v>
       </c>
       <c r="E10" t="n">
-        <v>159410947</v>
+        <v>170666467</v>
       </c>
     </row>
     <row r="11">
@@ -908,11 +908,6 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Rate Shock Scenario</t>
-        </is>
-      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Change in NII (1Y Horizon)</t>
@@ -936,7 +931,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2265363.79</v>
+        <v>2308583.54</v>
       </c>
     </row>
     <row r="4">
@@ -946,7 +941,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-2265363.79</v>
+        <v>-2308583.54</v>
       </c>
     </row>
     <row r="5">
@@ -956,7 +951,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>226536379</v>
+        <v>230858354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>